<commit_message>
fixed history plot and added ability to get best lot
</commit_message>
<xml_diff>
--- a/excel_data/2019_data/Win19_wk1_S.xlsx
+++ b/excel_data/2019_data/Win19_wk1_S.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C61209-861F-435F-9217-7A4442DC46B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D5FC6-F412-42E2-84EF-6460FCC9416F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{01F7802F-1915-4E07-B416-371742B259AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -223,16 +223,6 @@
         <family val="2"/>
       </rPr>
       <t>P701</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Regents Parking Lots</t>
     </r>
   </si>
   <si>
@@ -965,7 +955,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -981,64 +971,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="K1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="L1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="N1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="O1" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="P1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="R1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="S1" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="42" t="s">
+      <c r="T1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="U1" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="V1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="W1" s="41" t="s">
         <v>41</v>
-      </c>
-      <c r="W1" s="41" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -1877,12 +1867,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.399999999999999">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:23">
+      <c r="A14" s="30"/>
+      <c r="B14" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>20</v>
       </c>
       <c r="C14" s="23">
         <v>578</v>
@@ -1948,12 +1936,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="17.399999999999999">
-      <c r="A15" s="10" t="s">
-        <v>19</v>
-      </c>
+    <row r="15" spans="1:23">
+      <c r="A15" s="10"/>
       <c r="B15" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="11">
         <v>184</v>
@@ -2022,7 +2008,7 @@
     <row r="16" spans="1:23">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="33">
         <v>241</v>

</xml_diff>

<commit_message>
Combine the data extraction method with the data cleaning method.
</commit_message>
<xml_diff>
--- a/excel_data/2019_data/Win19_wk1_S.xlsx
+++ b/excel_data/2019_data/Win19_wk1_S.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114FC14D-A3FD-4D18-8EB6-F58D3ED03EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C61209-861F-435F-9217-7A4442DC46B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{01F7802F-1915-4E07-B416-371742B259AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <r>
       <rPr>
@@ -223,6 +223,16 @@
         <family val="2"/>
       </rPr>
       <t>P701</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Regents Parking Lots</t>
     </r>
   </si>
   <si>
@@ -955,7 +965,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -971,64 +981,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M1" s="41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" s="42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R1" s="41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S1" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T1" s="40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U1" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V1" s="41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W1" s="41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -1867,10 +1877,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:23" ht="17.399999999999999">
+      <c r="A14" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="23">
         <v>578</v>
@@ -1936,10 +1948,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:23" ht="17.399999999999999">
+      <c r="A15" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="B15" s="26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="11">
         <v>184</v>
@@ -2008,7 +2022,7 @@
     <row r="16" spans="1:23">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="33">
         <v>241</v>

</xml_diff>

<commit_message>
fixed 2019 data issues
</commit_message>
<xml_diff>
--- a/excel_data/2019_data/Win19_wk1_S.xlsx
+++ b/excel_data/2019_data/Win19_wk1_S.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C61209-861F-435F-9217-7A4442DC46B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69142457-BE9A-49F2-B8DD-F3A9D9E488CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{01F7802F-1915-4E07-B416-371742B259AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -223,16 +223,6 @@
         <family val="2"/>
       </rPr>
       <t>P701</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Regents Parking Lots</t>
     </r>
   </si>
   <si>
@@ -965,7 +955,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -981,64 +971,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="K1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="L1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="N1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="O1" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="P1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="R1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="S1" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="42" t="s">
+      <c r="T1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="U1" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="V1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="W1" s="41" t="s">
         <v>41</v>
-      </c>
-      <c r="W1" s="41" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -1877,12 +1867,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.399999999999999">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:23">
+      <c r="A14" s="30"/>
+      <c r="B14" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>20</v>
       </c>
       <c r="C14" s="23">
         <v>578</v>
@@ -1948,12 +1936,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="17.399999999999999">
-      <c r="A15" s="10" t="s">
-        <v>19</v>
-      </c>
+    <row r="15" spans="1:23">
+      <c r="A15" s="10"/>
       <c r="B15" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="11">
         <v>184</v>
@@ -2022,7 +2008,7 @@
     <row r="16" spans="1:23">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="33">
         <v>241</v>

</xml_diff>